<commit_message>
Commands as sent to SSC on 23 November
</commit_message>
<xml_diff>
--- a/output/tables/figure1_data.xlsx
+++ b/output/tables/figure1_data.xlsx
@@ -93,10 +93,10 @@
         <v>850</v>
       </c>
       <c r="C2">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D2">
-        <v>0.99295774647887325</v>
+        <v>0.95774647887323938</v>
       </c>
     </row>
     <row r="3">
@@ -107,10 +107,10 @@
         <v>855</v>
       </c>
       <c r="C3">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D3">
-        <v>0.99295774647887325</v>
+        <v>0.95070422535211263</v>
       </c>
     </row>
     <row r="4">
@@ -121,10 +121,10 @@
         <v>860</v>
       </c>
       <c r="C4">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D4">
-        <v>0.99295774647887325</v>
+        <v>0.95070422535211263</v>
       </c>
     </row>
     <row r="5">
@@ -135,10 +135,10 @@
         <v>865</v>
       </c>
       <c r="C5">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D5">
-        <v>0.99295774647887325</v>
+        <v>0.95070422535211263</v>
       </c>
     </row>
     <row r="6">
@@ -149,10 +149,10 @@
         <v>870</v>
       </c>
       <c r="C6">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D6">
-        <v>0.99295774647887325</v>
+        <v>0.94366197183098588</v>
       </c>
     </row>
     <row r="7">
@@ -163,10 +163,10 @@
         <v>875</v>
       </c>
       <c r="C7">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D7">
-        <v>0.99295774647887325</v>
+        <v>0.94366197183098588</v>
       </c>
     </row>
     <row r="8">
@@ -177,10 +177,10 @@
         <v>880</v>
       </c>
       <c r="C8">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D8">
-        <v>0.99295774647887325</v>
+        <v>0.94366197183098588</v>
       </c>
     </row>
     <row r="9">
@@ -191,10 +191,10 @@
         <v>885</v>
       </c>
       <c r="C9">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D9">
-        <v>0.99295774647887325</v>
+        <v>0.93661971830985913</v>
       </c>
     </row>
     <row r="10">
@@ -205,10 +205,10 @@
         <v>890</v>
       </c>
       <c r="C10">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D10">
-        <v>0.99295774647887325</v>
+        <v>0.93661971830985913</v>
       </c>
     </row>
     <row r="11">
@@ -219,10 +219,10 @@
         <v>895</v>
       </c>
       <c r="C11">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D11">
-        <v>0.99295774647887325</v>
+        <v>0.93661971830985913</v>
       </c>
     </row>
     <row r="12">
@@ -233,10 +233,10 @@
         <v>900</v>
       </c>
       <c r="C12">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D12">
-        <v>0.99295774647887325</v>
+        <v>0.93661971830985913</v>
       </c>
     </row>
     <row r="13">
@@ -247,10 +247,10 @@
         <v>905</v>
       </c>
       <c r="C13">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D13">
-        <v>0.99295774647887325</v>
+        <v>0.92253521126760563</v>
       </c>
     </row>
     <row r="14">
@@ -261,10 +261,10 @@
         <v>910</v>
       </c>
       <c r="C14">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="D14">
-        <v>0.99295774647887325</v>
+        <v>0.91549295774647887</v>
       </c>
     </row>
     <row r="15">
@@ -275,10 +275,10 @@
         <v>915</v>
       </c>
       <c r="C15">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="D15">
-        <v>0.99295774647887325</v>
+        <v>0.89436619718309862</v>
       </c>
     </row>
     <row r="16">
@@ -289,10 +289,10 @@
         <v>920</v>
       </c>
       <c r="C16">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="D16">
-        <v>0.97887323943661975</v>
+        <v>0.89436619718309862</v>
       </c>
     </row>
     <row r="17">
@@ -303,10 +303,10 @@
         <v>925</v>
       </c>
       <c r="C17">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="D17">
-        <v>0.97887323943661975</v>
+        <v>0.89436619718309862</v>
       </c>
     </row>
     <row r="18">
@@ -317,10 +317,10 @@
         <v>930</v>
       </c>
       <c r="C18">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="D18">
-        <v>0.97887323943661975</v>
+        <v>0.89436619718309862</v>
       </c>
     </row>
     <row r="19">
@@ -331,10 +331,10 @@
         <v>935</v>
       </c>
       <c r="C19">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="D19">
-        <v>0.97887323943661975</v>
+        <v>0.88732394366197187</v>
       </c>
     </row>
     <row r="20">
@@ -345,10 +345,10 @@
         <v>940</v>
       </c>
       <c r="C20">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="D20">
-        <v>0.97887323943661975</v>
+        <v>0.86619718309859151</v>
       </c>
     </row>
     <row r="21">
@@ -359,10 +359,10 @@
         <v>945</v>
       </c>
       <c r="C21">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="D21">
-        <v>0.97887323943661975</v>
+        <v>0.83098591549295775</v>
       </c>
     </row>
     <row r="22">
@@ -373,10 +373,10 @@
         <v>950</v>
       </c>
       <c r="C22">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="D22">
-        <v>0.97887323943661975</v>
+        <v>0.83098591549295775</v>
       </c>
     </row>
     <row r="23">
@@ -387,10 +387,10 @@
         <v>955</v>
       </c>
       <c r="C23">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="D23">
-        <v>0.97887323943661975</v>
+        <v>0.823943661971831</v>
       </c>
     </row>
     <row r="24">
@@ -401,10 +401,10 @@
         <v>960</v>
       </c>
       <c r="C24">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="D24">
-        <v>0.97887323943661975</v>
+        <v>0.77464788732394363</v>
       </c>
     </row>
     <row r="25">
@@ -415,10 +415,10 @@
         <v>965</v>
       </c>
       <c r="C25">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="D25">
-        <v>0.97887323943661975</v>
+        <v>0.76760563380281688</v>
       </c>
     </row>
     <row r="26">
@@ -429,10 +429,10 @@
         <v>970</v>
       </c>
       <c r="C26">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="D26">
-        <v>0.97887323943661975</v>
+        <v>0.73943661971830987</v>
       </c>
     </row>
     <row r="27">
@@ -443,10 +443,10 @@
         <v>975</v>
       </c>
       <c r="C27">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="D27">
-        <v>0.97887323943661975</v>
+        <v>0.73239436619718312</v>
       </c>
     </row>
     <row r="28">
@@ -457,10 +457,10 @@
         <v>980</v>
       </c>
       <c r="C28">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="D28">
-        <v>0.971830985915493</v>
+        <v>0.71830985915492962</v>
       </c>
     </row>
     <row r="29">
@@ -471,10 +471,10 @@
         <v>985</v>
       </c>
       <c r="C29">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="D29">
-        <v>0.971830985915493</v>
+        <v>0.71830985915492962</v>
       </c>
     </row>
     <row r="30">
@@ -485,10 +485,10 @@
         <v>990</v>
       </c>
       <c r="C30">
-        <v>138</v>
+        <v>96</v>
       </c>
       <c r="D30">
-        <v>0.971830985915493</v>
+        <v>0.676056338028169</v>
       </c>
     </row>
     <row r="31">
@@ -499,10 +499,10 @@
         <v>995</v>
       </c>
       <c r="C31">
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="D31">
-        <v>0.971830985915493</v>
+        <v>0.66901408450704225</v>
       </c>
     </row>
     <row r="32">
@@ -513,10 +513,10 @@
         <v>1</v>
       </c>
       <c r="C32">
-        <v>129</v>
+        <v>14</v>
       </c>
       <c r="D32">
-        <v>0.90845070422535212</v>
+        <v>0.0985915492957746</v>
       </c>
     </row>
     <row r="33">
@@ -527,10 +527,10 @@
         <v>850</v>
       </c>
       <c r="C33">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D33">
-        <v>0.99295774647887325</v>
+        <v>0.96478873239436624</v>
       </c>
     </row>
     <row r="34">
@@ -541,10 +541,10 @@
         <v>855</v>
       </c>
       <c r="C34">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D34">
-        <v>0.99295774647887325</v>
+        <v>0.96478873239436624</v>
       </c>
     </row>
     <row r="35">
@@ -555,10 +555,10 @@
         <v>860</v>
       </c>
       <c r="C35">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D35">
-        <v>0.99295774647887325</v>
+        <v>0.96478873239436624</v>
       </c>
     </row>
     <row r="36">
@@ -569,10 +569,10 @@
         <v>865</v>
       </c>
       <c r="C36">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D36">
-        <v>0.99295774647887325</v>
+        <v>0.96478873239436624</v>
       </c>
     </row>
     <row r="37">
@@ -583,10 +583,10 @@
         <v>870</v>
       </c>
       <c r="C37">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D37">
-        <v>0.99295774647887325</v>
+        <v>0.95774647887323938</v>
       </c>
     </row>
     <row r="38">
@@ -597,10 +597,10 @@
         <v>875</v>
       </c>
       <c r="C38">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D38">
-        <v>0.99295774647887325</v>
+        <v>0.95774647887323938</v>
       </c>
     </row>
     <row r="39">
@@ -611,10 +611,10 @@
         <v>880</v>
       </c>
       <c r="C39">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D39">
-        <v>0.99295774647887325</v>
+        <v>0.95774647887323938</v>
       </c>
     </row>
     <row r="40">
@@ -625,10 +625,10 @@
         <v>885</v>
       </c>
       <c r="C40">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="D40">
-        <v>0.99295774647887325</v>
+        <v>0.93661971830985913</v>
       </c>
     </row>
     <row r="41">
@@ -639,10 +639,10 @@
         <v>890</v>
       </c>
       <c r="C41">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D41">
-        <v>0.99295774647887325</v>
+        <v>0.92957746478873238</v>
       </c>
     </row>
     <row r="42">
@@ -653,10 +653,10 @@
         <v>895</v>
       </c>
       <c r="C42">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D42">
-        <v>0.99295774647887325</v>
+        <v>0.92253521126760563</v>
       </c>
     </row>
     <row r="43">
@@ -667,10 +667,10 @@
         <v>900</v>
       </c>
       <c r="C43">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="D43">
-        <v>0.99295774647887325</v>
+        <v>0.90845070422535212</v>
       </c>
     </row>
     <row r="44">
@@ -681,10 +681,10 @@
         <v>905</v>
       </c>
       <c r="C44">
-        <v>141</v>
+        <v>99</v>
       </c>
       <c r="D44">
-        <v>0.99295774647887325</v>
+        <v>0.69718309859154926</v>
       </c>
     </row>
     <row r="45">
@@ -695,10 +695,10 @@
         <v>910</v>
       </c>
       <c r="C45">
-        <v>141</v>
+        <v>98</v>
       </c>
       <c r="D45">
-        <v>0.99295774647887325</v>
+        <v>0.6901408450704225</v>
       </c>
     </row>
     <row r="46">
@@ -709,10 +709,10 @@
         <v>915</v>
       </c>
       <c r="C46">
-        <v>141</v>
+        <v>97</v>
       </c>
       <c r="D46">
-        <v>0.99295774647887325</v>
+        <v>0.68309859154929575</v>
       </c>
     </row>
     <row r="47">
@@ -723,10 +723,10 @@
         <v>920</v>
       </c>
       <c r="C47">
-        <v>139</v>
+        <v>95</v>
       </c>
       <c r="D47">
-        <v>0.97887323943661975</v>
+        <v>0.66901408450704225</v>
       </c>
     </row>
     <row r="48">
@@ -737,10 +737,10 @@
         <v>925</v>
       </c>
       <c r="C48">
-        <v>139</v>
+        <v>94</v>
       </c>
       <c r="D48">
-        <v>0.97887323943661975</v>
+        <v>0.6619718309859155</v>
       </c>
     </row>
     <row r="49">
@@ -751,10 +751,10 @@
         <v>930</v>
       </c>
       <c r="C49">
-        <v>139</v>
+        <v>91</v>
       </c>
       <c r="D49">
-        <v>0.97887323943661975</v>
+        <v>0.64084507042253525</v>
       </c>
     </row>
     <row r="50">
@@ -765,10 +765,10 @@
         <v>935</v>
       </c>
       <c r="C50">
-        <v>139</v>
+        <v>89</v>
       </c>
       <c r="D50">
-        <v>0.97887323943661975</v>
+        <v>0.62676056338028174</v>
       </c>
     </row>
     <row r="51">
@@ -779,10 +779,10 @@
         <v>940</v>
       </c>
       <c r="C51">
-        <v>139</v>
+        <v>87</v>
       </c>
       <c r="D51">
-        <v>0.97887323943661975</v>
+        <v>0.61267605633802813</v>
       </c>
     </row>
     <row r="52">
@@ -793,10 +793,10 @@
         <v>945</v>
       </c>
       <c r="C52">
-        <v>139</v>
+        <v>84</v>
       </c>
       <c r="D52">
-        <v>0.97887323943661975</v>
+        <v>0.59154929577464788</v>
       </c>
     </row>
     <row r="53">
@@ -807,10 +807,10 @@
         <v>950</v>
       </c>
       <c r="C53">
-        <v>139</v>
+        <v>82</v>
       </c>
       <c r="D53">
-        <v>0.97887323943661975</v>
+        <v>0.57746478873239437</v>
       </c>
     </row>
     <row r="54">
@@ -821,10 +821,10 @@
         <v>955</v>
       </c>
       <c r="C54">
-        <v>139</v>
+        <v>76</v>
       </c>
       <c r="D54">
-        <v>0.97887323943661975</v>
+        <v>0.53521126760563376</v>
       </c>
     </row>
     <row r="55">
@@ -835,10 +835,10 @@
         <v>960</v>
       </c>
       <c r="C55">
-        <v>139</v>
+        <v>13</v>
       </c>
       <c r="D55">
-        <v>0.97887323943661975</v>
+        <v>0.091549295774647904</v>
       </c>
     </row>
     <row r="56">
@@ -849,10 +849,10 @@
         <v>965</v>
       </c>
       <c r="C56">
-        <v>139</v>
+        <v>9</v>
       </c>
       <c r="D56">
-        <v>0.97887323943661975</v>
+        <v>0.063380281690140802</v>
       </c>
     </row>
     <row r="57">
@@ -863,10 +863,10 @@
         <v>970</v>
       </c>
       <c r="C57">
-        <v>139</v>
+        <v>9</v>
       </c>
       <c r="D57">
-        <v>0.97887323943661975</v>
+        <v>0.063380281690140802</v>
       </c>
     </row>
     <row r="58">
@@ -877,10 +877,10 @@
         <v>975</v>
       </c>
       <c r="C58">
-        <v>138</v>
+        <v>5</v>
       </c>
       <c r="D58">
-        <v>0.971830985915493</v>
+        <v>0.035211267605633798</v>
       </c>
     </row>
     <row r="59">
@@ -891,10 +891,10 @@
         <v>980</v>
       </c>
       <c r="C59">
-        <v>138</v>
+        <v>5</v>
       </c>
       <c r="D59">
-        <v>0.971830985915493</v>
+        <v>0.035211267605633798</v>
       </c>
     </row>
     <row r="60">
@@ -905,10 +905,10 @@
         <v>985</v>
       </c>
       <c r="C60">
-        <v>138</v>
+        <v>3</v>
       </c>
       <c r="D60">
-        <v>0.971830985915493</v>
+        <v>0.021126760563380299</v>
       </c>
     </row>
     <row r="61">
@@ -919,10 +919,10 @@
         <v>990</v>
       </c>
       <c r="C61">
-        <v>138</v>
+        <v>1</v>
       </c>
       <c r="D61">
-        <v>0.971830985915493</v>
+        <v>0.0070422535211267998</v>
       </c>
     </row>
     <row r="62">
@@ -933,10 +933,10 @@
         <v>995</v>
       </c>
       <c r="C62">
-        <v>138</v>
+        <v>1</v>
       </c>
       <c r="D62">
-        <v>0.971830985915493</v>
+        <v>0.0070422535211267998</v>
       </c>
     </row>
     <row r="63">
@@ -947,10 +947,10 @@
         <v>1</v>
       </c>
       <c r="C63">
-        <v>129</v>
+        <v>1</v>
       </c>
       <c r="D63">
-        <v>0.90845070422535212</v>
+        <v>0.0070422535211267998</v>
       </c>
     </row>
     <row r="64">
@@ -1395,10 +1395,10 @@
         <v>850</v>
       </c>
       <c r="C95">
-        <v>141</v>
+        <v>75</v>
       </c>
       <c r="D95">
-        <v>0.99295774647887325</v>
+        <v>0.528169014084507</v>
       </c>
     </row>
     <row r="96">
@@ -1409,10 +1409,10 @@
         <v>855</v>
       </c>
       <c r="C96">
-        <v>141</v>
+        <v>75</v>
       </c>
       <c r="D96">
-        <v>0.99295774647887325</v>
+        <v>0.528169014084507</v>
       </c>
     </row>
     <row r="97">
@@ -1423,10 +1423,10 @@
         <v>860</v>
       </c>
       <c r="C97">
-        <v>141</v>
+        <v>75</v>
       </c>
       <c r="D97">
-        <v>0.99295774647887325</v>
+        <v>0.528169014084507</v>
       </c>
     </row>
     <row r="98">
@@ -1437,10 +1437,10 @@
         <v>865</v>
       </c>
       <c r="C98">
-        <v>141</v>
+        <v>75</v>
       </c>
       <c r="D98">
-        <v>0.99295774647887325</v>
+        <v>0.528169014084507</v>
       </c>
     </row>
     <row r="99">
@@ -1451,10 +1451,10 @@
         <v>870</v>
       </c>
       <c r="C99">
-        <v>141</v>
+        <v>75</v>
       </c>
       <c r="D99">
-        <v>0.99295774647887325</v>
+        <v>0.528169014084507</v>
       </c>
     </row>
     <row r="100">
@@ -1465,10 +1465,10 @@
         <v>875</v>
       </c>
       <c r="C100">
-        <v>141</v>
+        <v>75</v>
       </c>
       <c r="D100">
-        <v>0.99295774647887325</v>
+        <v>0.528169014084507</v>
       </c>
     </row>
     <row r="101">
@@ -1479,10 +1479,10 @@
         <v>880</v>
       </c>
       <c r="C101">
-        <v>141</v>
+        <v>70</v>
       </c>
       <c r="D101">
-        <v>0.99295774647887325</v>
+        <v>0.49295774647887319</v>
       </c>
     </row>
     <row r="102">
@@ -1493,10 +1493,10 @@
         <v>885</v>
       </c>
       <c r="C102">
-        <v>141</v>
+        <v>70</v>
       </c>
       <c r="D102">
-        <v>0.99295774647887325</v>
+        <v>0.49295774647887319</v>
       </c>
     </row>
     <row r="103">
@@ -1507,10 +1507,10 @@
         <v>890</v>
       </c>
       <c r="C103">
-        <v>141</v>
+        <v>70</v>
       </c>
       <c r="D103">
-        <v>0.99295774647887325</v>
+        <v>0.49295774647887319</v>
       </c>
     </row>
     <row r="104">
@@ -1521,10 +1521,10 @@
         <v>895</v>
       </c>
       <c r="C104">
-        <v>141</v>
+        <v>70</v>
       </c>
       <c r="D104">
-        <v>0.99295774647887325</v>
+        <v>0.49295774647887319</v>
       </c>
     </row>
     <row r="105">
@@ -1535,10 +1535,10 @@
         <v>900</v>
       </c>
       <c r="C105">
-        <v>141</v>
+        <v>69</v>
       </c>
       <c r="D105">
-        <v>0.99295774647887325</v>
+        <v>0.4859154929577465</v>
       </c>
     </row>
     <row r="106">
@@ -1549,10 +1549,10 @@
         <v>905</v>
       </c>
       <c r="C106">
-        <v>141</v>
+        <v>65</v>
       </c>
       <c r="D106">
-        <v>0.99295774647887325</v>
+        <v>0.45774647887323938</v>
       </c>
     </row>
     <row r="107">
@@ -1563,10 +1563,10 @@
         <v>910</v>
       </c>
       <c r="C107">
-        <v>141</v>
+        <v>65</v>
       </c>
       <c r="D107">
-        <v>0.99295774647887325</v>
+        <v>0.45774647887323938</v>
       </c>
     </row>
     <row r="108">
@@ -1577,10 +1577,10 @@
         <v>915</v>
       </c>
       <c r="C108">
-        <v>141</v>
+        <v>65</v>
       </c>
       <c r="D108">
-        <v>0.99295774647887325</v>
+        <v>0.45774647887323938</v>
       </c>
     </row>
     <row r="109">
@@ -1591,10 +1591,10 @@
         <v>920</v>
       </c>
       <c r="C109">
-        <v>139</v>
+        <v>65</v>
       </c>
       <c r="D109">
-        <v>0.97887323943661975</v>
+        <v>0.45774647887323938</v>
       </c>
     </row>
     <row r="110">
@@ -1605,10 +1605,10 @@
         <v>925</v>
       </c>
       <c r="C110">
-        <v>139</v>
+        <v>65</v>
       </c>
       <c r="D110">
-        <v>0.97887323943661975</v>
+        <v>0.45774647887323938</v>
       </c>
     </row>
     <row r="111">
@@ -1619,10 +1619,10 @@
         <v>930</v>
       </c>
       <c r="C111">
-        <v>139</v>
+        <v>65</v>
       </c>
       <c r="D111">
-        <v>0.97887323943661975</v>
+        <v>0.45774647887323938</v>
       </c>
     </row>
     <row r="112">
@@ -1633,10 +1633,10 @@
         <v>935</v>
       </c>
       <c r="C112">
-        <v>139</v>
+        <v>64</v>
       </c>
       <c r="D112">
-        <v>0.97887323943661975</v>
+        <v>0.45070422535211269</v>
       </c>
     </row>
     <row r="113">
@@ -1647,10 +1647,10 @@
         <v>940</v>
       </c>
       <c r="C113">
-        <v>139</v>
+        <v>64</v>
       </c>
       <c r="D113">
-        <v>0.97887323943661975</v>
+        <v>0.45070422535211269</v>
       </c>
     </row>
     <row r="114">
@@ -1661,10 +1661,10 @@
         <v>945</v>
       </c>
       <c r="C114">
-        <v>139</v>
+        <v>64</v>
       </c>
       <c r="D114">
-        <v>0.97887323943661975</v>
+        <v>0.45070422535211269</v>
       </c>
     </row>
     <row r="115">
@@ -1675,10 +1675,10 @@
         <v>950</v>
       </c>
       <c r="C115">
-        <v>139</v>
+        <v>63</v>
       </c>
       <c r="D115">
-        <v>0.97887323943661975</v>
+        <v>0.44366197183098588</v>
       </c>
     </row>
     <row r="116">
@@ -1689,10 +1689,10 @@
         <v>955</v>
       </c>
       <c r="C116">
-        <v>139</v>
+        <v>63</v>
       </c>
       <c r="D116">
-        <v>0.97887323943661975</v>
+        <v>0.44366197183098588</v>
       </c>
     </row>
     <row r="117">
@@ -1703,10 +1703,10 @@
         <v>960</v>
       </c>
       <c r="C117">
-        <v>139</v>
+        <v>63</v>
       </c>
       <c r="D117">
-        <v>0.97887323943661975</v>
+        <v>0.44366197183098588</v>
       </c>
     </row>
     <row r="118">
@@ -1717,10 +1717,10 @@
         <v>965</v>
       </c>
       <c r="C118">
-        <v>139</v>
+        <v>63</v>
       </c>
       <c r="D118">
-        <v>0.97887323943661975</v>
+        <v>0.44366197183098588</v>
       </c>
     </row>
     <row r="119">
@@ -1731,10 +1731,10 @@
         <v>970</v>
       </c>
       <c r="C119">
-        <v>139</v>
+        <v>63</v>
       </c>
       <c r="D119">
-        <v>0.97887323943661975</v>
+        <v>0.44366197183098588</v>
       </c>
     </row>
     <row r="120">
@@ -1745,10 +1745,10 @@
         <v>975</v>
       </c>
       <c r="C120">
-        <v>138</v>
+        <v>63</v>
       </c>
       <c r="D120">
-        <v>0.971830985915493</v>
+        <v>0.44366197183098588</v>
       </c>
     </row>
     <row r="121">
@@ -1759,10 +1759,10 @@
         <v>980</v>
       </c>
       <c r="C121">
-        <v>138</v>
+        <v>62</v>
       </c>
       <c r="D121">
-        <v>0.971830985915493</v>
+        <v>0.43661971830985907</v>
       </c>
     </row>
     <row r="122">
@@ -1773,10 +1773,10 @@
         <v>985</v>
       </c>
       <c r="C122">
-        <v>138</v>
+        <v>62</v>
       </c>
       <c r="D122">
-        <v>0.971830985915493</v>
+        <v>0.43661971830985907</v>
       </c>
     </row>
     <row r="123">
@@ -1787,10 +1787,10 @@
         <v>990</v>
       </c>
       <c r="C123">
-        <v>138</v>
+        <v>62</v>
       </c>
       <c r="D123">
-        <v>0.971830985915493</v>
+        <v>0.43661971830985907</v>
       </c>
     </row>
     <row r="124">
@@ -1801,10 +1801,10 @@
         <v>995</v>
       </c>
       <c r="C124">
-        <v>138</v>
+        <v>62</v>
       </c>
       <c r="D124">
-        <v>0.971830985915493</v>
+        <v>0.43661971830985907</v>
       </c>
     </row>
     <row r="125">
@@ -1815,879 +1815,383 @@
         <v>1</v>
       </c>
       <c r="C125">
-        <v>129</v>
+        <v>46</v>
       </c>
       <c r="D125">
-        <v>0.90845070422535212</v>
+        <v>0.323943661971831</v>
       </c>
     </row>
     <row r="126">
-      <c r="A126">
-        <v>5</v>
-      </c>
-      <c r="B126">
-        <v>850</v>
-      </c>
-      <c r="C126">
-        <v>136</v>
-      </c>
-      <c r="D126">
-        <v>0.95774647887323938</v>
-      </c>
+      <c r="A126"/>
+      <c r="B126"/>
+      <c r="C126"/>
+      <c r="D126"/>
     </row>
     <row r="127">
-      <c r="A127">
-        <v>5</v>
-      </c>
-      <c r="B127">
-        <v>855</v>
-      </c>
-      <c r="C127">
-        <v>135</v>
-      </c>
-      <c r="D127">
-        <v>0.95070422535211263</v>
-      </c>
+      <c r="A127"/>
+      <c r="B127"/>
+      <c r="C127"/>
+      <c r="D127"/>
     </row>
     <row r="128">
-      <c r="A128">
-        <v>5</v>
-      </c>
-      <c r="B128">
-        <v>860</v>
-      </c>
-      <c r="C128">
-        <v>135</v>
-      </c>
-      <c r="D128">
-        <v>0.95070422535211263</v>
-      </c>
+      <c r="A128"/>
+      <c r="B128"/>
+      <c r="C128"/>
+      <c r="D128"/>
     </row>
     <row r="129">
-      <c r="A129">
-        <v>5</v>
-      </c>
-      <c r="B129">
-        <v>865</v>
-      </c>
-      <c r="C129">
-        <v>135</v>
-      </c>
-      <c r="D129">
-        <v>0.95070422535211263</v>
-      </c>
+      <c r="A129"/>
+      <c r="B129"/>
+      <c r="C129"/>
+      <c r="D129"/>
     </row>
     <row r="130">
-      <c r="A130">
-        <v>5</v>
-      </c>
-      <c r="B130">
-        <v>870</v>
-      </c>
-      <c r="C130">
-        <v>134</v>
-      </c>
-      <c r="D130">
-        <v>0.94366197183098588</v>
-      </c>
+      <c r="A130"/>
+      <c r="B130"/>
+      <c r="C130"/>
+      <c r="D130"/>
     </row>
     <row r="131">
-      <c r="A131">
-        <v>5</v>
-      </c>
-      <c r="B131">
-        <v>875</v>
-      </c>
-      <c r="C131">
-        <v>134</v>
-      </c>
-      <c r="D131">
-        <v>0.94366197183098588</v>
-      </c>
+      <c r="A131"/>
+      <c r="B131"/>
+      <c r="C131"/>
+      <c r="D131"/>
     </row>
     <row r="132">
-      <c r="A132">
-        <v>5</v>
-      </c>
-      <c r="B132">
-        <v>880</v>
-      </c>
-      <c r="C132">
-        <v>134</v>
-      </c>
-      <c r="D132">
-        <v>0.94366197183098588</v>
-      </c>
+      <c r="A132"/>
+      <c r="B132"/>
+      <c r="C132"/>
+      <c r="D132"/>
     </row>
     <row r="133">
-      <c r="A133">
-        <v>5</v>
-      </c>
-      <c r="B133">
-        <v>885</v>
-      </c>
-      <c r="C133">
-        <v>133</v>
-      </c>
-      <c r="D133">
-        <v>0.93661971830985913</v>
-      </c>
+      <c r="A133"/>
+      <c r="B133"/>
+      <c r="C133"/>
+      <c r="D133"/>
     </row>
     <row r="134">
-      <c r="A134">
-        <v>5</v>
-      </c>
-      <c r="B134">
-        <v>890</v>
-      </c>
-      <c r="C134">
-        <v>133</v>
-      </c>
-      <c r="D134">
-        <v>0.93661971830985913</v>
-      </c>
+      <c r="A134"/>
+      <c r="B134"/>
+      <c r="C134"/>
+      <c r="D134"/>
     </row>
     <row r="135">
-      <c r="A135">
-        <v>5</v>
-      </c>
-      <c r="B135">
-        <v>895</v>
-      </c>
-      <c r="C135">
-        <v>133</v>
-      </c>
-      <c r="D135">
-        <v>0.93661971830985913</v>
-      </c>
+      <c r="A135"/>
+      <c r="B135"/>
+      <c r="C135"/>
+      <c r="D135"/>
     </row>
     <row r="136">
-      <c r="A136">
-        <v>5</v>
-      </c>
-      <c r="B136">
-        <v>900</v>
-      </c>
-      <c r="C136">
-        <v>133</v>
-      </c>
-      <c r="D136">
-        <v>0.93661971830985913</v>
-      </c>
+      <c r="A136"/>
+      <c r="B136"/>
+      <c r="C136"/>
+      <c r="D136"/>
     </row>
     <row r="137">
-      <c r="A137">
-        <v>5</v>
-      </c>
-      <c r="B137">
-        <v>905</v>
-      </c>
-      <c r="C137">
-        <v>131</v>
-      </c>
-      <c r="D137">
-        <v>0.92253521126760563</v>
-      </c>
+      <c r="A137"/>
+      <c r="B137"/>
+      <c r="C137"/>
+      <c r="D137"/>
     </row>
     <row r="138">
-      <c r="A138">
-        <v>5</v>
-      </c>
-      <c r="B138">
-        <v>910</v>
-      </c>
-      <c r="C138">
-        <v>130</v>
-      </c>
-      <c r="D138">
-        <v>0.91549295774647887</v>
-      </c>
+      <c r="A138"/>
+      <c r="B138"/>
+      <c r="C138"/>
+      <c r="D138"/>
     </row>
     <row r="139">
-      <c r="A139">
-        <v>5</v>
-      </c>
-      <c r="B139">
-        <v>915</v>
-      </c>
-      <c r="C139">
-        <v>127</v>
-      </c>
-      <c r="D139">
-        <v>0.89436619718309862</v>
-      </c>
+      <c r="A139"/>
+      <c r="B139"/>
+      <c r="C139"/>
+      <c r="D139"/>
     </row>
     <row r="140">
-      <c r="A140">
-        <v>5</v>
-      </c>
-      <c r="B140">
-        <v>920</v>
-      </c>
-      <c r="C140">
-        <v>127</v>
-      </c>
-      <c r="D140">
-        <v>0.89436619718309862</v>
-      </c>
+      <c r="A140"/>
+      <c r="B140"/>
+      <c r="C140"/>
+      <c r="D140"/>
     </row>
     <row r="141">
-      <c r="A141">
-        <v>5</v>
-      </c>
-      <c r="B141">
-        <v>925</v>
-      </c>
-      <c r="C141">
-        <v>127</v>
-      </c>
-      <c r="D141">
-        <v>0.89436619718309862</v>
-      </c>
+      <c r="A141"/>
+      <c r="B141"/>
+      <c r="C141"/>
+      <c r="D141"/>
     </row>
     <row r="142">
-      <c r="A142">
-        <v>5</v>
-      </c>
-      <c r="B142">
-        <v>930</v>
-      </c>
-      <c r="C142">
-        <v>127</v>
-      </c>
-      <c r="D142">
-        <v>0.89436619718309862</v>
-      </c>
+      <c r="A142"/>
+      <c r="B142"/>
+      <c r="C142"/>
+      <c r="D142"/>
     </row>
     <row r="143">
-      <c r="A143">
-        <v>5</v>
-      </c>
-      <c r="B143">
-        <v>935</v>
-      </c>
-      <c r="C143">
-        <v>126</v>
-      </c>
-      <c r="D143">
-        <v>0.88732394366197187</v>
-      </c>
+      <c r="A143"/>
+      <c r="B143"/>
+      <c r="C143"/>
+      <c r="D143"/>
     </row>
     <row r="144">
-      <c r="A144">
-        <v>5</v>
-      </c>
-      <c r="B144">
-        <v>940</v>
-      </c>
-      <c r="C144">
-        <v>123</v>
-      </c>
-      <c r="D144">
-        <v>0.86619718309859151</v>
-      </c>
+      <c r="A144"/>
+      <c r="B144"/>
+      <c r="C144"/>
+      <c r="D144"/>
     </row>
     <row r="145">
-      <c r="A145">
-        <v>5</v>
-      </c>
-      <c r="B145">
-        <v>945</v>
-      </c>
-      <c r="C145">
-        <v>118</v>
-      </c>
-      <c r="D145">
-        <v>0.83098591549295775</v>
-      </c>
+      <c r="A145"/>
+      <c r="B145"/>
+      <c r="C145"/>
+      <c r="D145"/>
     </row>
     <row r="146">
-      <c r="A146">
-        <v>5</v>
-      </c>
-      <c r="B146">
-        <v>950</v>
-      </c>
-      <c r="C146">
-        <v>118</v>
-      </c>
-      <c r="D146">
-        <v>0.83098591549295775</v>
-      </c>
+      <c r="A146"/>
+      <c r="B146"/>
+      <c r="C146"/>
+      <c r="D146"/>
     </row>
     <row r="147">
-      <c r="A147">
-        <v>5</v>
-      </c>
-      <c r="B147">
-        <v>955</v>
-      </c>
-      <c r="C147">
-        <v>117</v>
-      </c>
-      <c r="D147">
-        <v>0.823943661971831</v>
-      </c>
+      <c r="A147"/>
+      <c r="B147"/>
+      <c r="C147"/>
+      <c r="D147"/>
     </row>
     <row r="148">
-      <c r="A148">
-        <v>5</v>
-      </c>
-      <c r="B148">
-        <v>960</v>
-      </c>
-      <c r="C148">
-        <v>110</v>
-      </c>
-      <c r="D148">
-        <v>0.77464788732394363</v>
-      </c>
+      <c r="A148"/>
+      <c r="B148"/>
+      <c r="C148"/>
+      <c r="D148"/>
     </row>
     <row r="149">
-      <c r="A149">
-        <v>5</v>
-      </c>
-      <c r="B149">
-        <v>965</v>
-      </c>
-      <c r="C149">
-        <v>109</v>
-      </c>
-      <c r="D149">
-        <v>0.76760563380281688</v>
-      </c>
+      <c r="A149"/>
+      <c r="B149"/>
+      <c r="C149"/>
+      <c r="D149"/>
     </row>
     <row r="150">
-      <c r="A150">
-        <v>5</v>
-      </c>
-      <c r="B150">
-        <v>970</v>
-      </c>
-      <c r="C150">
-        <v>105</v>
-      </c>
-      <c r="D150">
-        <v>0.73943661971830987</v>
-      </c>
+      <c r="A150"/>
+      <c r="B150"/>
+      <c r="C150"/>
+      <c r="D150"/>
     </row>
     <row r="151">
-      <c r="A151">
-        <v>5</v>
-      </c>
-      <c r="B151">
-        <v>975</v>
-      </c>
-      <c r="C151">
-        <v>104</v>
-      </c>
-      <c r="D151">
-        <v>0.73239436619718312</v>
-      </c>
+      <c r="A151"/>
+      <c r="B151"/>
+      <c r="C151"/>
+      <c r="D151"/>
     </row>
     <row r="152">
-      <c r="A152">
-        <v>5</v>
-      </c>
-      <c r="B152">
-        <v>980</v>
-      </c>
-      <c r="C152">
-        <v>102</v>
-      </c>
-      <c r="D152">
-        <v>0.71830985915492962</v>
-      </c>
+      <c r="A152"/>
+      <c r="B152"/>
+      <c r="C152"/>
+      <c r="D152"/>
     </row>
     <row r="153">
-      <c r="A153">
-        <v>5</v>
-      </c>
-      <c r="B153">
-        <v>985</v>
-      </c>
-      <c r="C153">
-        <v>102</v>
-      </c>
-      <c r="D153">
-        <v>0.71830985915492962</v>
-      </c>
+      <c r="A153"/>
+      <c r="B153"/>
+      <c r="C153"/>
+      <c r="D153"/>
     </row>
     <row r="154">
-      <c r="A154">
-        <v>5</v>
-      </c>
-      <c r="B154">
-        <v>990</v>
-      </c>
-      <c r="C154">
-        <v>96</v>
-      </c>
-      <c r="D154">
-        <v>0.676056338028169</v>
-      </c>
+      <c r="A154"/>
+      <c r="B154"/>
+      <c r="C154"/>
+      <c r="D154"/>
     </row>
     <row r="155">
-      <c r="A155">
-        <v>5</v>
-      </c>
-      <c r="B155">
-        <v>995</v>
-      </c>
-      <c r="C155">
-        <v>95</v>
-      </c>
-      <c r="D155">
-        <v>0.66901408450704225</v>
-      </c>
+      <c r="A155"/>
+      <c r="B155"/>
+      <c r="C155"/>
+      <c r="D155"/>
     </row>
     <row r="156">
-      <c r="A156">
-        <v>5</v>
-      </c>
-      <c r="B156">
-        <v>1</v>
-      </c>
-      <c r="C156">
-        <v>14</v>
-      </c>
-      <c r="D156">
-        <v>0.0985915492957746</v>
-      </c>
+      <c r="A156"/>
+      <c r="B156"/>
+      <c r="C156"/>
+      <c r="D156"/>
     </row>
     <row r="157">
-      <c r="A157">
-        <v>6</v>
-      </c>
-      <c r="B157">
-        <v>850</v>
-      </c>
-      <c r="C157">
-        <v>137</v>
-      </c>
-      <c r="D157">
-        <v>0.96478873239436624</v>
-      </c>
+      <c r="A157"/>
+      <c r="B157"/>
+      <c r="C157"/>
+      <c r="D157"/>
     </row>
     <row r="158">
-      <c r="A158">
-        <v>6</v>
-      </c>
-      <c r="B158">
-        <v>855</v>
-      </c>
-      <c r="C158">
-        <v>137</v>
-      </c>
-      <c r="D158">
-        <v>0.96478873239436624</v>
-      </c>
+      <c r="A158"/>
+      <c r="B158"/>
+      <c r="C158"/>
+      <c r="D158"/>
     </row>
     <row r="159">
-      <c r="A159">
-        <v>6</v>
-      </c>
-      <c r="B159">
-        <v>860</v>
-      </c>
-      <c r="C159">
-        <v>137</v>
-      </c>
-      <c r="D159">
-        <v>0.96478873239436624</v>
-      </c>
+      <c r="A159"/>
+      <c r="B159"/>
+      <c r="C159"/>
+      <c r="D159"/>
     </row>
     <row r="160">
-      <c r="A160">
-        <v>6</v>
-      </c>
-      <c r="B160">
-        <v>865</v>
-      </c>
-      <c r="C160">
-        <v>137</v>
-      </c>
-      <c r="D160">
-        <v>0.96478873239436624</v>
-      </c>
+      <c r="A160"/>
+      <c r="B160"/>
+      <c r="C160"/>
+      <c r="D160"/>
     </row>
     <row r="161">
-      <c r="A161">
-        <v>6</v>
-      </c>
-      <c r="B161">
-        <v>870</v>
-      </c>
-      <c r="C161">
-        <v>136</v>
-      </c>
-      <c r="D161">
-        <v>0.95774647887323938</v>
-      </c>
+      <c r="A161"/>
+      <c r="B161"/>
+      <c r="C161"/>
+      <c r="D161"/>
     </row>
     <row r="162">
-      <c r="A162">
-        <v>6</v>
-      </c>
-      <c r="B162">
-        <v>875</v>
-      </c>
-      <c r="C162">
-        <v>136</v>
-      </c>
-      <c r="D162">
-        <v>0.95774647887323938</v>
-      </c>
+      <c r="A162"/>
+      <c r="B162"/>
+      <c r="C162"/>
+      <c r="D162"/>
     </row>
     <row r="163">
-      <c r="A163">
-        <v>6</v>
-      </c>
-      <c r="B163">
-        <v>880</v>
-      </c>
-      <c r="C163">
-        <v>136</v>
-      </c>
-      <c r="D163">
-        <v>0.95774647887323938</v>
-      </c>
+      <c r="A163"/>
+      <c r="B163"/>
+      <c r="C163"/>
+      <c r="D163"/>
     </row>
     <row r="164">
-      <c r="A164">
-        <v>6</v>
-      </c>
-      <c r="B164">
-        <v>885</v>
-      </c>
-      <c r="C164">
-        <v>133</v>
-      </c>
-      <c r="D164">
-        <v>0.93661971830985913</v>
-      </c>
+      <c r="A164"/>
+      <c r="B164"/>
+      <c r="C164"/>
+      <c r="D164"/>
     </row>
     <row r="165">
-      <c r="A165">
-        <v>6</v>
-      </c>
-      <c r="B165">
-        <v>890</v>
-      </c>
-      <c r="C165">
-        <v>132</v>
-      </c>
-      <c r="D165">
-        <v>0.92957746478873238</v>
-      </c>
+      <c r="A165"/>
+      <c r="B165"/>
+      <c r="C165"/>
+      <c r="D165"/>
     </row>
     <row r="166">
-      <c r="A166">
-        <v>6</v>
-      </c>
-      <c r="B166">
-        <v>895</v>
-      </c>
-      <c r="C166">
-        <v>131</v>
-      </c>
-      <c r="D166">
-        <v>0.92253521126760563</v>
-      </c>
+      <c r="A166"/>
+      <c r="B166"/>
+      <c r="C166"/>
+      <c r="D166"/>
     </row>
     <row r="167">
-      <c r="A167">
-        <v>6</v>
-      </c>
-      <c r="B167">
-        <v>900</v>
-      </c>
-      <c r="C167">
-        <v>129</v>
-      </c>
-      <c r="D167">
-        <v>0.90845070422535212</v>
-      </c>
+      <c r="A167"/>
+      <c r="B167"/>
+      <c r="C167"/>
+      <c r="D167"/>
     </row>
     <row r="168">
-      <c r="A168">
-        <v>6</v>
-      </c>
-      <c r="B168">
-        <v>905</v>
-      </c>
-      <c r="C168">
-        <v>99</v>
-      </c>
-      <c r="D168">
-        <v>0.69718309859154926</v>
-      </c>
+      <c r="A168"/>
+      <c r="B168"/>
+      <c r="C168"/>
+      <c r="D168"/>
     </row>
     <row r="169">
-      <c r="A169">
-        <v>6</v>
-      </c>
-      <c r="B169">
-        <v>910</v>
-      </c>
-      <c r="C169">
-        <v>98</v>
-      </c>
-      <c r="D169">
-        <v>0.6901408450704225</v>
-      </c>
+      <c r="A169"/>
+      <c r="B169"/>
+      <c r="C169"/>
+      <c r="D169"/>
     </row>
     <row r="170">
-      <c r="A170">
-        <v>6</v>
-      </c>
-      <c r="B170">
-        <v>915</v>
-      </c>
-      <c r="C170">
-        <v>97</v>
-      </c>
-      <c r="D170">
-        <v>0.68309859154929575</v>
-      </c>
+      <c r="A170"/>
+      <c r="B170"/>
+      <c r="C170"/>
+      <c r="D170"/>
     </row>
     <row r="171">
-      <c r="A171">
-        <v>6</v>
-      </c>
-      <c r="B171">
-        <v>920</v>
-      </c>
-      <c r="C171">
-        <v>95</v>
-      </c>
-      <c r="D171">
-        <v>0.66901408450704225</v>
-      </c>
+      <c r="A171"/>
+      <c r="B171"/>
+      <c r="C171"/>
+      <c r="D171"/>
     </row>
     <row r="172">
-      <c r="A172">
-        <v>6</v>
-      </c>
-      <c r="B172">
-        <v>925</v>
-      </c>
-      <c r="C172">
-        <v>94</v>
-      </c>
-      <c r="D172">
-        <v>0.6619718309859155</v>
-      </c>
+      <c r="A172"/>
+      <c r="B172"/>
+      <c r="C172"/>
+      <c r="D172"/>
     </row>
     <row r="173">
-      <c r="A173">
-        <v>6</v>
-      </c>
-      <c r="B173">
-        <v>930</v>
-      </c>
-      <c r="C173">
-        <v>91</v>
-      </c>
-      <c r="D173">
-        <v>0.64084507042253525</v>
-      </c>
+      <c r="A173"/>
+      <c r="B173"/>
+      <c r="C173"/>
+      <c r="D173"/>
     </row>
     <row r="174">
-      <c r="A174">
-        <v>6</v>
-      </c>
-      <c r="B174">
-        <v>935</v>
-      </c>
-      <c r="C174">
-        <v>89</v>
-      </c>
-      <c r="D174">
-        <v>0.62676056338028174</v>
-      </c>
+      <c r="A174"/>
+      <c r="B174"/>
+      <c r="C174"/>
+      <c r="D174"/>
     </row>
     <row r="175">
-      <c r="A175">
-        <v>6</v>
-      </c>
-      <c r="B175">
-        <v>940</v>
-      </c>
-      <c r="C175">
-        <v>87</v>
-      </c>
-      <c r="D175">
-        <v>0.61267605633802813</v>
-      </c>
+      <c r="A175"/>
+      <c r="B175"/>
+      <c r="C175"/>
+      <c r="D175"/>
     </row>
     <row r="176">
-      <c r="A176">
-        <v>6</v>
-      </c>
-      <c r="B176">
-        <v>945</v>
-      </c>
-      <c r="C176">
-        <v>84</v>
-      </c>
-      <c r="D176">
-        <v>0.59154929577464788</v>
-      </c>
+      <c r="A176"/>
+      <c r="B176"/>
+      <c r="C176"/>
+      <c r="D176"/>
     </row>
     <row r="177">
-      <c r="A177">
-        <v>6</v>
-      </c>
-      <c r="B177">
-        <v>950</v>
-      </c>
-      <c r="C177">
-        <v>82</v>
-      </c>
-      <c r="D177">
-        <v>0.57746478873239437</v>
-      </c>
+      <c r="A177"/>
+      <c r="B177"/>
+      <c r="C177"/>
+      <c r="D177"/>
     </row>
     <row r="178">
-      <c r="A178">
-        <v>6</v>
-      </c>
-      <c r="B178">
-        <v>955</v>
-      </c>
-      <c r="C178">
-        <v>76</v>
-      </c>
-      <c r="D178">
-        <v>0.53521126760563376</v>
-      </c>
+      <c r="A178"/>
+      <c r="B178"/>
+      <c r="C178"/>
+      <c r="D178"/>
     </row>
     <row r="179">
-      <c r="A179">
-        <v>6</v>
-      </c>
-      <c r="B179">
-        <v>960</v>
-      </c>
-      <c r="C179">
-        <v>13</v>
-      </c>
-      <c r="D179">
-        <v>0.091549295774647904</v>
-      </c>
+      <c r="A179"/>
+      <c r="B179"/>
+      <c r="C179"/>
+      <c r="D179"/>
     </row>
     <row r="180">
-      <c r="A180">
-        <v>6</v>
-      </c>
-      <c r="B180">
-        <v>965</v>
-      </c>
-      <c r="C180">
-        <v>9</v>
-      </c>
-      <c r="D180">
-        <v>0.063380281690140802</v>
-      </c>
+      <c r="A180"/>
+      <c r="B180"/>
+      <c r="C180"/>
+      <c r="D180"/>
     </row>
     <row r="181">
-      <c r="A181">
-        <v>6</v>
-      </c>
-      <c r="B181">
-        <v>970</v>
-      </c>
-      <c r="C181">
-        <v>9</v>
-      </c>
-      <c r="D181">
-        <v>0.063380281690140802</v>
-      </c>
+      <c r="A181"/>
+      <c r="B181"/>
+      <c r="C181"/>
+      <c r="D181"/>
     </row>
     <row r="182">
-      <c r="A182">
-        <v>6</v>
-      </c>
-      <c r="B182">
-        <v>975</v>
-      </c>
-      <c r="C182">
-        <v>5</v>
-      </c>
-      <c r="D182">
-        <v>0.035211267605633798</v>
-      </c>
+      <c r="A182"/>
+      <c r="B182"/>
+      <c r="C182"/>
+      <c r="D182"/>
     </row>
     <row r="183">
-      <c r="A183">
-        <v>6</v>
-      </c>
-      <c r="B183">
-        <v>980</v>
-      </c>
-      <c r="C183">
-        <v>5</v>
-      </c>
-      <c r="D183">
-        <v>0.035211267605633798</v>
-      </c>
+      <c r="A183"/>
+      <c r="B183"/>
+      <c r="C183"/>
+      <c r="D183"/>
     </row>
     <row r="184">
-      <c r="A184">
-        <v>6</v>
-      </c>
-      <c r="B184">
-        <v>985</v>
-      </c>
-      <c r="C184">
-        <v>3</v>
-      </c>
-      <c r="D184">
-        <v>0.021126760563380299</v>
-      </c>
+      <c r="A184"/>
+      <c r="B184"/>
+      <c r="C184"/>
+      <c r="D184"/>
     </row>
     <row r="185">
-      <c r="A185">
-        <v>6</v>
-      </c>
-      <c r="B185">
-        <v>990</v>
-      </c>
-      <c r="C185">
-        <v>1</v>
-      </c>
-      <c r="D185">
-        <v>0.0070422535211267998</v>
-      </c>
+      <c r="A185"/>
+      <c r="B185"/>
+      <c r="C185"/>
+      <c r="D185"/>
     </row>
     <row r="186">
-      <c r="A186">
-        <v>6</v>
-      </c>
-      <c r="B186">
-        <v>995</v>
-      </c>
-      <c r="C186">
-        <v>1</v>
-      </c>
-      <c r="D186">
-        <v>0.0070422535211267998</v>
-      </c>
+      <c r="A186"/>
+      <c r="B186"/>
+      <c r="C186"/>
+      <c r="D186"/>
     </row>
     <row r="187">
-      <c r="A187">
-        <v>6</v>
-      </c>
-      <c r="B187">
-        <v>1</v>
-      </c>
-      <c r="C187">
-        <v>1</v>
-      </c>
-      <c r="D187">
-        <v>0.0070422535211267998</v>
-      </c>
+      <c r="A187"/>
+      <c r="B187"/>
+      <c r="C187"/>
+      <c r="D187"/>
     </row>
     <row r="188">
       <c r="A188"/>

</xml_diff>